<commit_message>
Changed wireframing to priority 1
</commit_message>
<xml_diff>
--- a/Documentation/Product Backlog2.xlsx
+++ b/Documentation/Product Backlog2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\daniel.bowen\source\repos\Kanrail\5153-Ethics_Game\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4350D404-A346-4C2E-BBFC-B881E16FD2C1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{185643CF-257C-4B4D-8FED-9470ECC6EED9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2730" yWindow="2730" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -419,7 +419,7 @@
   <dimension ref="A1:I1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -686,7 +686,7 @@
         <v>37</v>
       </c>
       <c r="C11" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>38</v>

</xml_diff>